<commit_message>
PUR 4 automation test cases code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PUR/PUR_TestData.xlsx
+++ b/src/test/resources/TestData/PUR/PUR_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9580F71D-1E69-4258-ADDA-4056211C5E28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323DBF7F-1687-4BBE-B95B-99CFCB17FBBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="15255" windowHeight="6255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15255" windowHeight="6255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
   <si>
     <t>UserName</t>
   </si>
@@ -383,6 +383,15 @@
   </si>
   <si>
     <t>Primary</t>
+  </si>
+  <si>
+    <t>promocode</t>
+  </si>
+  <si>
+    <t>PUR20</t>
+  </si>
+  <si>
+    <t>PromoCode</t>
   </si>
 </sst>
 </file>
@@ -753,12 +762,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AM9" sqref="AM9"/>
+      <selection pane="bottomLeft" activeCell="AP26" sqref="AP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,9 +805,10 @@
     <col min="37" max="37" width="16.85546875" customWidth="1"/>
     <col min="38" max="38" width="15.42578125" customWidth="1"/>
     <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -916,8 +926,11 @@
       <c r="AM1" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN1" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -937,7 +950,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -957,7 +970,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -977,7 +990,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1026,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1034,7 +1047,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1055,7 +1068,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1075,7 +1088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1137,7 +1150,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1196,7 +1209,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1234,7 +1247,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1242,7 +1255,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1262,7 +1275,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1270,7 +1283,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1278,7 +1291,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1286,7 +1299,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -1294,7 +1307,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1311,7 +1324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1319,7 +1332,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1345,7 +1358,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -1383,7 +1396,7 @@
       </c>
       <c r="U22" s="10"/>
     </row>
-    <row r="23" spans="1:36" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -1403,7 +1416,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -1423,7 +1436,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -1432,6 +1445,14 @@
       </c>
       <c r="AJ25">
         <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN26" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PUR 5 New Expansion Test cases, PUR helper, PUR TestData and PUR xml
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PUR/PUR_TestData.xlsx
+++ b/src/test/resources/TestData/PUR/PUR_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323DBF7F-1687-4BBE-B95B-99CFCB17FBBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6CC83D-FF8E-4839-97A2-0DAD474AFF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15255" windowHeight="6255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
   <si>
     <t>UserName</t>
   </si>
@@ -392,6 +392,18 @@
   </si>
   <si>
     <t>PromoCode</t>
+  </si>
+  <si>
+    <t>compareproduct</t>
+  </si>
+  <si>
+    <t>Abcd12345</t>
+  </si>
+  <si>
+    <t>vivekvickky168@gmail.com</t>
+  </si>
+  <si>
+    <t>PUR PLUS Pitcher Filter</t>
   </si>
 </sst>
 </file>
@@ -762,12 +774,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN26"/>
+  <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AP26" sqref="AP26"/>
+      <selection pane="bottomLeft" activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,9 +818,10 @@
     <col min="38" max="38" width="15.42578125" customWidth="1"/>
     <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -929,8 +942,11 @@
       <c r="AN1" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO1" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -938,7 +954,7 @@
         <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
         <v>113</v>
@@ -947,10 +963,10 @@
         <v>95</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -970,7 +986,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -990,7 +1006,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1026,7 +1042,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1063,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1068,7 +1084,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1087,8 +1103,11 @@
       <c r="V8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1150,7 +1169,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1209,7 +1228,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1247,7 +1266,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1255,7 +1274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1275,7 +1294,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1283,7 +1302,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1291,7 +1310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1457,23 +1476,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
-    <hyperlink ref="U8" r:id="rId4" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
-    <hyperlink ref="V8" r:id="rId5" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
-    <hyperlink ref="F4" r:id="rId7" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
-    <hyperlink ref="F18" r:id="rId8" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
-    <hyperlink ref="F20" r:id="rId9" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
-    <hyperlink ref="F21" r:id="rId10" xr:uid="{9FBE7ED1-9FD9-45D4-B0EF-56EFE1DA2EBB}"/>
-    <hyperlink ref="B4" r:id="rId11" xr:uid="{3A274BA2-8B1D-45EA-B7AF-85F9D6EF8D70}"/>
-    <hyperlink ref="F5" r:id="rId12" xr:uid="{48B2F49A-712D-4845-9E3A-B3049EAFB524}"/>
-    <hyperlink ref="B3" r:id="rId13" xr:uid="{ED21BB6E-4719-47CD-B2F3-C497C3D84EFA}"/>
-    <hyperlink ref="C3" r:id="rId14" xr:uid="{279423C6-76FC-4C99-B0BC-FF614C1868CF}"/>
-    <hyperlink ref="F3" r:id="rId15" xr:uid="{84B10434-ED9C-4084-8E96-7905FE54D8BC}"/>
-    <hyperlink ref="F11" r:id="rId16" xr:uid="{C8E2DB01-3056-4D89-827B-25213284A8F6}"/>
-    <hyperlink ref="F10" r:id="rId17" xr:uid="{AE5D2C1F-B288-418A-B785-A2DA9EB26F5A}"/>
+    <hyperlink ref="C2" r:id="rId1" display="Vihaan@2018" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="U8" r:id="rId2" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
+    <hyperlink ref="V8" r:id="rId3" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
+    <hyperlink ref="F18" r:id="rId6" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
+    <hyperlink ref="F20" r:id="rId7" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
+    <hyperlink ref="F21" r:id="rId8" xr:uid="{9FBE7ED1-9FD9-45D4-B0EF-56EFE1DA2EBB}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{3A274BA2-8B1D-45EA-B7AF-85F9D6EF8D70}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{48B2F49A-712D-4845-9E3A-B3049EAFB524}"/>
+    <hyperlink ref="B3" r:id="rId11" xr:uid="{ED21BB6E-4719-47CD-B2F3-C497C3D84EFA}"/>
+    <hyperlink ref="C3" r:id="rId12" xr:uid="{279423C6-76FC-4C99-B0BC-FF614C1868CF}"/>
+    <hyperlink ref="F3" r:id="rId13" xr:uid="{84B10434-ED9C-4084-8E96-7905FE54D8BC}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{C8E2DB01-3056-4D89-827B-25213284A8F6}"/>
+    <hyperlink ref="F10" r:id="rId15" xr:uid="{AE5D2C1F-B288-418A-B785-A2DA9EB26F5A}"/>
+    <hyperlink ref="B2" r:id="rId16" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
+    <hyperlink ref="F2" r:id="rId17" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId18"/>

</xml_diff>

<commit_message>
PUR expansion test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/PUR/PUR_TestData.xlsx
+++ b/src/test/resources/TestData/PUR/PUR_TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6CC83D-FF8E-4839-97A2-0DAD474AFF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3912129D-2524-4F23-B28C-707DFF79F1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="1230" windowWidth="14430" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="136">
   <si>
     <t>UserName</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Chiruvella</t>
   </si>
   <si>
-    <t>harish.chiruvella1@gmail.com</t>
-  </si>
-  <si>
     <t>Harish!123</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>Revlon Hair Tools &lt;Revlon@r1.dotdigital-email.com&gt;</t>
   </si>
   <si>
-    <t>Harish Chiruvella &lt;harish.chiruvella1@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Your Password Reset Request</t>
   </si>
   <si>
@@ -404,6 +398,36 @@
   </si>
   <si>
     <t>PUR PLUS Pitcher Filter</t>
+  </si>
+  <si>
+    <t>saiteja@gmail.com</t>
+  </si>
+  <si>
+    <t>Harish Chiruvella &lt;saiteja@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>DifferentBillandshipping</t>
+  </si>
+  <si>
+    <t>New Address</t>
+  </si>
+  <si>
+    <t>No_Tax_Address</t>
+  </si>
+  <si>
+    <t>saitejakasturi@gmail.com</t>
+  </si>
+  <si>
+    <t>7257 Randall Mill Court</t>
+  </si>
+  <si>
+    <t>Westminster Station</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Newaddress</t>
   </si>
 </sst>
 </file>
@@ -774,12 +798,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO26"/>
+  <dimension ref="A1:AP28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AO8" sqref="AO8"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,39 +813,38 @@
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="46.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="9.140625" style="5"/>
-    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.85546875" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" customWidth="1"/>
-    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.7109375" customWidth="1"/>
-    <col min="41" max="41" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="9.140625" style="5"/>
+    <col min="29" max="29" width="23" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.85546875" customWidth="1"/>
+    <col min="39" max="39" width="15.42578125" customWidth="1"/>
+    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" customWidth="1"/>
+    <col min="42" max="42" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -844,10 +867,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
@@ -859,178 +882,181 @@
         <v>12</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="O1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="AE1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>83</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
       </c>
       <c r="K5" t="s">
         <v>7</v>
@@ -1038,78 +1064,78 @@
       <c r="L5">
         <v>12345</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>9898989899</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" s="6">
+        <v>4444424444444440</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>2023</v>
+      </c>
+      <c r="R6" t="s">
+        <v>97</v>
+      </c>
+      <c r="S6" s="3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="O7" t="s">
+        <v>94</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>2021</v>
+      </c>
+      <c r="R7" t="s">
         <v>96</v>
       </c>
-      <c r="O6" s="6">
-        <v>4444424444444440</v>
-      </c>
-      <c r="P6" s="8">
-        <v>2023</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>99</v>
-      </c>
-      <c r="R6" s="3">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="N7" t="s">
-        <v>96</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="P7" s="8">
-        <v>2021</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>98</v>
-      </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="T8" t="s">
+        <v>112</v>
+      </c>
+      <c r="U8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="S8" t="s">
-        <v>114</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="V8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -1118,60 +1144,60 @@
         <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
         <v>37</v>
-      </c>
-      <c r="I9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" t="s">
-        <v>38</v>
       </c>
       <c r="L9">
         <v>12345</v>
       </c>
-      <c r="M9" s="3">
+      <c r="N9" s="3">
         <v>9898989899</v>
       </c>
-      <c r="S9" t="s">
-        <v>118</v>
-      </c>
       <c r="T9" t="s">
+        <v>116</v>
+      </c>
+      <c r="U9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9">
+        <v>12341</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>2020</v>
+      </c>
+      <c r="AM9">
+        <v>44000000438</v>
+      </c>
+      <c r="AN9">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>43</v>
-      </c>
-      <c r="W9">
-        <v>12341</v>
-      </c>
-      <c r="X9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>5</v>
-      </c>
-      <c r="Z9" s="5">
-        <v>6</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>2020</v>
-      </c>
-      <c r="AL9">
-        <v>44000000438</v>
-      </c>
-      <c r="AM9">
-        <v>9898989898</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -1180,57 +1206,57 @@
         <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" t="s">
         <v>37</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" t="s">
-        <v>38</v>
       </c>
       <c r="L10">
         <v>12345</v>
       </c>
-      <c r="M10" s="3">
+      <c r="N10" s="3">
         <v>9898989899</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
+        <v>112</v>
+      </c>
+      <c r="U10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10">
+        <v>12341</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z10" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="T10" t="s">
-        <v>43</v>
-      </c>
-      <c r="W10">
-        <v>12341</v>
-      </c>
-      <c r="X10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y10" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="Z10" s="5">
+      <c r="AA10" s="5">
         <v>6</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AB10" s="5">
         <v>2020</v>
       </c>
-      <c r="AK10" s="13">
+      <c r="AL10" s="13">
         <v>43955</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1239,50 +1265,51 @@
         <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
         <v>54</v>
       </c>
-      <c r="H11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>55</v>
       </c>
-      <c r="K11" t="s">
-        <v>56</v>
-      </c>
       <c r="L11" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="M11" s="3">
+        <v>71</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="3">
         <v>9898989899</v>
       </c>
-      <c r="S11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" t="s">
         <v>49</v>
       </c>
-      <c r="S12" t="s">
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>53</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
@@ -1291,213 +1318,280 @@
         <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="T14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>57</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>58</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T16" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="S16" s="7" t="s">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>65</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="AB18" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y20"/>
+        <v>126</v>
+      </c>
       <c r="Z20"/>
       <c r="AA20"/>
-      <c r="AE20" t="s">
+      <c r="AB20"/>
+      <c r="AF20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH20" t="s">
         <v>77</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AI20" t="s">
         <v>78</v>
       </c>
-      <c r="AG20" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21">
+        <v>126</v>
+      </c>
+      <c r="N21">
         <v>9898989899</v>
       </c>
-      <c r="X21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="Y21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O22" t="s">
+        <v>101</v>
+      </c>
+      <c r="P22" s="9">
+        <v>371449635398431</v>
+      </c>
+      <c r="Q22">
+        <v>2023</v>
+      </c>
+      <c r="R22" t="s">
+        <v>97</v>
+      </c>
+      <c r="S22">
+        <v>3456</v>
+      </c>
+      <c r="V22" s="10"/>
+    </row>
+    <row r="23" spans="1:41" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="O23" t="s">
+        <v>103</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q23">
+        <v>2023</v>
+      </c>
+      <c r="R23" t="s">
+        <v>97</v>
+      </c>
+      <c r="S23">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>100</v>
       </c>
-      <c r="N22" t="s">
-        <v>103</v>
-      </c>
-      <c r="O22" s="9">
-        <v>371449635398431</v>
-      </c>
-      <c r="P22">
+      <c r="O24" t="s">
+        <v>102</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q24">
         <v>2023</v>
       </c>
-      <c r="Q22" t="s">
-        <v>99</v>
-      </c>
-      <c r="R22">
-        <v>3456</v>
-      </c>
-      <c r="U22" s="10"/>
-    </row>
-    <row r="23" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>101</v>
-      </c>
-      <c r="N23" t="s">
-        <v>105</v>
-      </c>
-      <c r="O23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="P23">
-        <v>2023</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>99</v>
-      </c>
-      <c r="R23">
+      <c r="R24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S24">
         <v>345</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>102</v>
-      </c>
-      <c r="N24" t="s">
-        <v>104</v>
-      </c>
-      <c r="O24" s="12" t="s">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
-      <c r="P24">
-        <v>2023</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>99</v>
-      </c>
-      <c r="R24">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI25" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ25">
+      <c r="AJ25" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN26" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="AO26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27">
+        <v>6492</v>
+      </c>
+      <c r="M27" t="s">
+        <v>129</v>
+      </c>
+      <c r="N27">
+        <v>9898989899</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" t="s">
+        <v>133</v>
+      </c>
+      <c r="K28" t="s">
+        <v>134</v>
+      </c>
+      <c r="L28">
+        <v>5159</v>
+      </c>
+      <c r="N28">
+        <v>9898989899</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Vihaan@2018" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="U8" r:id="rId2" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
-    <hyperlink ref="V8" r:id="rId3" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
-    <hyperlink ref="F9" r:id="rId4" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
+    <hyperlink ref="V8" r:id="rId2" xr:uid="{4220B5CE-425B-448F-BB9D-BD038E3AEC51}"/>
+    <hyperlink ref="W8" r:id="rId3" xr:uid="{0726E8FB-FA32-40D5-9D64-FEBF7414A6F6}"/>
+    <hyperlink ref="F9" r:id="rId4" display="harish.chiruvella1@gmail.com" xr:uid="{3CE92D6D-283B-48AA-B301-460813BB2679}"/>
     <hyperlink ref="F4" r:id="rId5" xr:uid="{B44C5DE3-CF91-4BC6-8D84-760826E2DF8E}"/>
-    <hyperlink ref="F18" r:id="rId6" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
-    <hyperlink ref="F20" r:id="rId7" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
-    <hyperlink ref="F21" r:id="rId8" xr:uid="{9FBE7ED1-9FD9-45D4-B0EF-56EFE1DA2EBB}"/>
+    <hyperlink ref="F18" r:id="rId6" display="harish.chiruvella1@gmail.com" xr:uid="{30E3E29B-A01C-4FE7-97FE-3E7B31458DE1}"/>
+    <hyperlink ref="F20" r:id="rId7" display="harish.chiruvella1@gmail.com" xr:uid="{A4043BC6-567C-4555-83DA-28B8577169BC}"/>
+    <hyperlink ref="F21" r:id="rId8" display="harish.chiruvella1@gmail.com" xr:uid="{9FBE7ED1-9FD9-45D4-B0EF-56EFE1DA2EBB}"/>
     <hyperlink ref="B4" r:id="rId9" xr:uid="{3A274BA2-8B1D-45EA-B7AF-85F9D6EF8D70}"/>
     <hyperlink ref="F5" r:id="rId10" xr:uid="{48B2F49A-712D-4845-9E3A-B3049EAFB524}"/>
     <hyperlink ref="B3" r:id="rId11" xr:uid="{ED21BB6E-4719-47CD-B2F3-C497C3D84EFA}"/>
     <hyperlink ref="C3" r:id="rId12" xr:uid="{279423C6-76FC-4C99-B0BC-FF614C1868CF}"/>
     <hyperlink ref="F3" r:id="rId13" xr:uid="{84B10434-ED9C-4084-8E96-7905FE54D8BC}"/>
-    <hyperlink ref="F11" r:id="rId14" xr:uid="{C8E2DB01-3056-4D89-827B-25213284A8F6}"/>
-    <hyperlink ref="F10" r:id="rId15" xr:uid="{AE5D2C1F-B288-418A-B785-A2DA9EB26F5A}"/>
+    <hyperlink ref="F11" r:id="rId14" display="harish.chiruvella1@gmail.com" xr:uid="{C8E2DB01-3056-4D89-827B-25213284A8F6}"/>
+    <hyperlink ref="F10" r:id="rId15" display="harish.chiruvella1@gmail.com" xr:uid="{AE5D2C1F-B288-418A-B785-A2DA9EB26F5A}"/>
     <hyperlink ref="B2" r:id="rId16" xr:uid="{F914D97D-9AB4-479F-B5C1-406A7A6E213A}"/>
     <hyperlink ref="F2" r:id="rId17" xr:uid="{654737CF-7ECC-40EB-8F54-3F2A1D6BA9EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId18"/>
   <ignoredErrors>
-    <ignoredError sqref="O7" numberStoredAsText="1"/>
+    <ignoredError sqref="P7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>